<commit_message>
feat: Update candidate data and enhance configuration management
- Updated candidate information in JSON and Excel files.
- Added a default configuration file creation mechanism.
- Improved logging functionality and ensured output directories are created.
- Enhanced the PyInstaller configuration for building the executable.
- Added PowerShell script for building the executable with options for browser selection.
- Created a batch script to run the executable and open logs.
- Included example configuration file for user reference.
</commit_message>
<xml_diff>
--- a/output/candidates/excel/curriculos_coletados.xlsx
+++ b/output/candidates/excel/curriculos_coletados.xlsx
@@ -458,1085 +458,1113 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Marciene Santos</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>Marcia Kerlianny</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>30 anos, Casada - São Paulo, São Paulo - CONJUNTO PROMORAR SAPOPEMBA</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(11) 94001-8070</t>
+          <t>(84) 99896-7952</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>masantos0824@gmail.com</t>
+          <t>kerliannymarita@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Luiz Filipe Della Volpe</t>
+          <t>LUCIANA LIMA ROQUE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>47 anos, Casado - São Paulo, São Paulo - JARDIM REPRESA</t>
+          <t>39 anos, Casada - São Paulo, São Paulo - CIDADE SAO MATEUS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(11) 96340-3104</t>
+          <t>(11) 93905-3575</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>vadiagemeletronika@gmail.com</t>
+          <t>roquelima2@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Marcelo Segecs</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>Giovanna de Melo Novaes Gonçalves</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>São Paulo, São Paulo</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(11) 95499-6263</t>
+          <t>(11) 97734-2613</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>segecs@hotmail.com</t>
+          <t>giovannamelong@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pedro Henrique de Sousa</t>
+          <t>Thifany Rodrigues Cordeiro</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24 anos, Solteiro - São Paulo, São Paulo - jardim lajeado</t>
+          <t>21 anos, Solteira - São Paulo, São Paulo - VILA CARMOSINA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(11) 98115-3778</t>
+          <t>(11) 96942-5187</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>pehsouza12@gmail.com</t>
+          <t>thifanycordeiro1306@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Marcos Imbimbo</t>
+          <t>Gabriela de Oliveira Herculano</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>47 anos, Casado - São Paulo, São Paulo - Vila Prudente</t>
+          <t>29 anos, Solteira - São Paulo, São Paulo - JD NOSSA SENHORA DO CARMO</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(11) 97633-6005</t>
+          <t>(11) 91342-7366
+(11) 94070-3110</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>maimbimbo@yahoo.com.br</t>
+          <t>gabrieladeoliveiraherculano@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Joyce Kelly Barbosa de Moura Branco</t>
+          <t>Tomás Souza</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>29 anos, São Paulo, São Paulo - JARDIM AEROPORTO II</t>
+          <t>23 anos, Solteiro - São Paulo, São Paulo - Jabaquara</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(11) 95197-7281</t>
+          <t>(11) 99334-4099</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>joymoura16@gmail.com</t>
+          <t>prodtoggz@icloud.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Victor da Silva Fernandes</t>
+          <t>Patrick Lima Santos</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>26 anos, Solteiro - São Paulo, São Paulo - Balneário São José</t>
+          <t>35 anos, Casado - São Paulo, São Paulo - Cangaíba</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(11) 96911-5001</t>
+          <t>(11) 94514-1963</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>victordasilvafernandes@gmail.com</t>
+          <t>patricstss@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Milene de Jesus Silva</t>
+          <t>Celio Faustino da Silva</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>34 anos, Solteira - São Paulo, São Paulo - Paraisópolis</t>
+          <t>39 anos, Solteiro - São Paulo, São Paulo - Jardim Ester</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>(11) 93907-5767</t>
+          <t>(11) 98239-9680
+(11) 98239-9680</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>mi.jsilvah@gmail.com</t>
+          <t>celiocfs2010@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Vitoria Rossi Valentim</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+          <t>MARIANNE RODRIGUES MOREIRA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>São Paulo, São Paulo</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>(11) 99027-1286</t>
+          <t>(11) 98724-4611</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>rossivitoria14@gmail.com</t>
+          <t>rodriguesmarianne902@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ednei D'Angelo</t>
+          <t>Matheus Aparecido Ferreira</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>55 anos, Divorciado - São Paulo, São Paulo - JARDIM BELA VISTA</t>
+          <t>30 anos, Solteiro - São Paulo, São Paulo - Vila São Geraldo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>(11) 98875-0008</t>
+          <t>(11) 94971-4338</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ednei.dangelo@gmail.com</t>
+          <t>aoomath25@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Rodrigo Villa Rosa</t>
+          <t>Riquelme</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>45 anos, Casado - São Paulo, São Paulo - Nossa Senhora do Ó</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>(11) 94394-8401</t>
+          <t>(11) 91330-1844</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>rodrigovillarosa@gmail.com</t>
+          <t>rickraiquone@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Fernanda Bueno</t>
+          <t>Renan Ramos Torezan</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>31 anos, Solteira - São Paulo, São Paulo - JARDIM BOTUCATU</t>
+          <t>37 anos, Solteiro - São Paulo, São Paulo - CIDADE LIDER</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>(11) 94701-1944
-(11) 94701-1944</t>
+          <t>(11) 95713-6795</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ferbueno994@gmail.com</t>
+          <t>renantorezan30@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Yvan Santos</t>
+          <t>Ana Carolina Sousa Pereira Forte</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>29 anos, Casado - São Paulo, São Paulo - Centro</t>
+          <t>25 anos, Solteira - São Paulo, São Paulo - Vila Bela</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>(11) 91416-1710</t>
+          <t>(11) 99166-4054</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>yvan.bep2013@gmail.com</t>
+          <t>carolfortee@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Suelen Pereira de Sousa</t>
+          <t>Marcos E S Martini</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>38 anos, Solteira - São Paulo, São Paulo - Parque Santo Antônio</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>(11) 98344-5957</t>
+          <t>(11) 91327-0174</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>suelensousa87@hotmail.com</t>
+          <t>smartini1806@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ezequiel Alves Costa</t>
+          <t>Gustavo Fernandes da Costa</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>27 anos, Solteiro - São Paulo, São Paulo - Parque América</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>(11) 98995-9636</t>
+          <t>(11) 91684-7297</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ezequielportinnari@hotmail.com</t>
+          <t>gustavofernandescosta2023@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Suzi Marinho</t>
+          <t>Yasmin costa</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17 anos e 9 meses</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>(11) 94986-8597
-(11) 94986-8597</t>
+          <t>(11) 92011-2713</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>smarinho@hotmail.com.br</t>
+          <t>cyasminpaixao2404@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jéssica Batista Soares</t>
+          <t>Sandra Vasconcelos</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>34 anos, Solteira - São Paulo, São Paulo - VILA BELA VISTA</t>
+          <t>50 anos, Solteira - São Paulo, São Paulo - NOSSA SENHORA DO O</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>(11) 98166-5914</t>
+          <t>(11) 94856-8888
+(11) 94856-8888</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Jessicabatista3467@gmail.com</t>
+          <t>arqsandrabelanger@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Camila Oliveira Noguchi</t>
+          <t>Joelson de Almeida Santos</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17 anos, Solteira - São Paulo, São Paulo - Cidade Tiradentes</t>
+          <t>41 anos, Casado - São Paulo, São Paulo - VILA TAQUARI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>(11) 95484-4144</t>
+          <t>(11) 96805-8590</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>camilaoliveiranoguchi1508@gmail.com</t>
+          <t>jbunidos29@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Desirêe Soares Ferreira</t>
+          <t>yasmim</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>32 anos, Solteira - São Paulo, São Paulo - Parada inglesa Zona norte</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>(11) 98318-7305</t>
+          <t>(11) 94554-6694</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>desireefgestora@gmail.com</t>
+          <t>yasminreiis002@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ester ribeiro da silva</t>
+          <t>Shirley Belarmino da Silva</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>25 anos, Solteira - São Paulo, São Paulo - jardim Bartira</t>
+          <t>48 anos, Solteira - São Paulo, São Paulo - VILA SAO FRANCISCO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>(11) 93002-5851</t>
+          <t>(11) 94728-4788</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>esterribeirosilvaers@gmail.com</t>
+          <t>shirleysilva123@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Eishyla Dantas da Silva</t>
+          <t>Maiane Magalhães da Silva</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>28 anos, Solteira - São Paulo, São Paulo - Jardim São Jorge</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>(11) 96343-3396</t>
+          <t>(71) 98421-3825</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>eishylad@gmail.com</t>
+          <t>maianemagalhaess27@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Natália Costa</t>
+          <t>Carlos Daniel do Amor Divino Rios</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>37 anos, Solteira - São Paulo, São Paulo - Vila Nova Manchester</t>
+          <t>22 anos, Solteiro - São Paulo, São Paulo - Jardim Monte Verde</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>(11) 99799-1317</t>
+          <t>(11) 96444-3202
+(11) 96444-3202</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>natie_c@hotmail.com</t>
+          <t>carlosdanieldivino@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Francyroger Freitas Santos</t>
+          <t>Aline Duarte Buccedi</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>51 anos, Casado - São Paulo, São Paulo - PARQUE MANDAQUI</t>
+          <t>44 anos, Divorciada - São Paulo, São Paulo - VILA PRUDENTE</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>(11) 97040-8866</t>
+          <t>(11) 91832-2277
+(22) 99930-2277</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>roggersantos74@gmail.com</t>
+          <t>alinenf@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Beatriz Lopes Da Silva Paulo</t>
+          <t>Mariana Becker De Jorge</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>23 anos, Solteira - São Paulo, São Paulo - São paulo</t>
+          <t>19 anos, Solteira - São Paulo, São Paulo - BRAS</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>(11) 99449-5114</t>
+          <t>(11) 98340-1413</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Beeatrizlopesss@gmail.com</t>
+          <t>Beckerdejorgemariana@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Diego Vinicius</t>
+          <t>Ruan vitor pinheiro alves da silva</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>29 anos, São Paulo, São Paulo - PARQUE NOVO LAR</t>
+          <t>22 anos, Solteiro - São Paulo, São Paulo - Jardim Nova Harmonia</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>(11) 94080-2277</t>
+          <t>(11) 96288-9140</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>galvao.diego.vinicius@gmail.com</t>
+          <t>ruan2003.v@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Antônio Carlos Magalhães</t>
+          <t>Vitoria Sotero da Silva Pereira</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>55 anos, Casado - São Paulo, São Paulo - JARDIM SANDRA MARIA</t>
+          <t>25 anos, Solteira - São Paulo, São Paulo - JARDIM AURELIO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>(11) 96538-6405</t>
+          <t>(83) 99832-5912
+(11) 9636-1288</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>45acmb@gmail.com</t>
+          <t>vitoriapereria26@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Aline Almeida Santos</t>
+          <t>Luna Barros Ribeiro</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>26 anos, Casada - São Paulo, São Paulo - Jardim Tango</t>
+          <t>24 anos, Solteira - São Paulo, São Paulo - VILA MORAES</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>(11) 98299-4716</t>
+          <t>(24) 98168-0227
+(11) 94829-1007</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>alinealmeida7140@gmail.com</t>
+          <t>lunabribeiro20@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Aline Melevski Marchetti</t>
+          <t>Maria Clara de Oliveira lima</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>38 anos, Solteira - São Paulo, São Paulo - VILA CALIFORNIA</t>
+          <t>20 anos, Solteira - São Paulo, São Paulo - Mooca</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>(13) 99791-3705</t>
+          <t>(11) 95496-0839</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>aline.marchetti1987@gmail.com</t>
+          <t>mlima6582@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Jardel cesar nogueira</t>
+          <t>SARA VITÓRIA DA SILVA MATOS</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>24 anos, Solteiro - São Paulo, São Paulo - Jardim Cambara</t>
+          <t>19 anos, Solteira - São Paulo, São Paulo - Vila Conde do Pinhal</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>(11) 99577-9113
-(31) 98710-9253</t>
+          <t>(19) 99867-0775</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>jardelcesarnogueira@hotmail.com</t>
+          <t>sarav.silvamatos@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Cristina Prado</t>
+          <t>Danielly Nair Batista Reis</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>São Paulo, São Paulo - VILA CARRAO</t>
+          <t>40 anos, Solteira - São Paulo, São Paulo - Osasco</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>(11) 98596-1283</t>
+          <t>(11) 99171-9614</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>crys_1707@outlook.com</t>
+          <t>daniellyreis02@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Carolina Mak Mud Gois</t>
+          <t>Eliane Alves de Carvalho</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>São Paulo, São Paulo</t>
+          <t>39 anos, Divorciada - São Paulo, São Paulo - VILA CONSTANCIA</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>(11) 98393-8261</t>
+          <t>(11) 98030-1744</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>carolinagoois.mak@outlook.com</t>
+          <t>elianecagidu@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lais Juarez</t>
+          <t>Mikaela da Silva santos</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>31 anos, Casada - São Paulo, São Paulo - VILA SANTA CLARA</t>
+          <t>24 anos, Solteira - São Paulo, São Paulo - cidade Tiradentes</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>(11) 98963-9254</t>
+          <t>(19) 99655-0945
+(19) 98133-6482</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>laisjuarez@gmail.com</t>
+          <t>Dmikaela644@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mariana Baptista Alves</t>
+          <t>Marluce Silva de Jesus</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31 anos, Solteira - São Paulo, São Paulo - Conjunto Residencial Jose Boni</t>
+          <t>33 anos, Solteira - São Paulo, São Paulo - VILA PRADO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>(11) 99236-1604
-(11) 99515-0318</t>
+          <t>(11) 95818-2730</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>mariana_bap_tista@hotmail.com</t>
+          <t>marluce_djesus@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Laura Oliveira da Silva</t>
+          <t>Geovanna Ribeiro Silva</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>27 anos, Solteira - São Paulo, São Paulo - PARQUE DAS PAINEIRAS</t>
+          <t>17 anos, Solteira - São Paulo, São Paulo - Itaim Paulista</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>(11) 99822-2030</t>
+          <t>(11) 96036-1252
+(11) 97634-7195</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>rh.lauraoliveira@gmail.com</t>
+          <t>geovannaribeirossilva@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Andrea Cristina da Silva</t>
+          <t>Pedro Henrique dos Santos Silva</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>46 anos, Solteira - São Paulo, São Paulo - Residencial Central Park Lapa</t>
+          <t>19 anos, Solteiro - São Paulo, São Paulo - Chácara Santo Antônio</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>(11) 99355-5740
-(11) 2776-6605</t>
+          <t>(11) 97591-7168</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>andreaariely3@gmail.com</t>
+          <t>phenriquess2611@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Diego Corrêa Nunes</t>
+          <t>Monica Godoi</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>37 anos, Solteiro - São Paulo, São Paulo - Jardim Umarizal</t>
+          <t>39 anos, Divorciada - São Paulo, São Paulo - VILA SILVA TELES</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>(11) 91648-8062</t>
+          <t>(11) 99118-6503</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>dcnunes@live.com</t>
+          <t>Monicagodoiplatero23@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Amanda Gomes dos Santos Lima</t>
+          <t>Isabelle Schneider</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>30 anos, Casada - São Paulo, São Paulo - Jardim Olinda</t>
+          <t>22 anos, Solteira - São Paulo, São Paulo - JARDIM PEDRO JOSE NUNES</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>(11) 98629-7771</t>
+          <t>(11) 94115-6793</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>amanda.silva.gomes@bol.com.br</t>
+          <t>isabelle11schneider@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Thalita Aires</t>
+          <t>Maria Eduarda Rocha Van Acker</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>22 anos, Solteira - São Paulo, São Paulo - JARDIM SANTA FE</t>
+          <t>21 anos, Solteira - São Paulo, São Paulo - Jordanopolis</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>(11) 98680-1516</t>
+          <t>(11) 95090-5643
+(11) 95131-3094</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>contatothalitaaires@gmail.com</t>
+          <t>dudarochaav@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jenniffer Cristina Inácio Vieira</t>
+          <t>Nathale Maciel Araujo</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>27 anos, Solteira - São Paulo, São Paulo - JARDIM DAS IMBUIAS</t>
+          <t>24 anos, Solteira - São Paulo, São Paulo - Jardim São Pedro</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>(11) 97897-0555
-(11) 5972-9816</t>
+          <t>(63) 99232-6053</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>jennifferinacio02@gmail.com</t>
+          <t>contatonathalimaciel@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>sandra b oliveira</t>
+          <t>Kaua silv88</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>58 anos, São Paulo, São Paulo - IPIRANGA</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>(11) 97464-1461</t>
+          <t>(11) 96215-2553</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>sandraboliveira@yahoo.com.br</t>
+          <t>damacenok750@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ellen Caroline Silva Viana</t>
+          <t>Gabriel cardoso</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>27 anos, Casada - São Paulo, São Paulo - JARDIM IRIS</t>
+          <t>22 anos, Solteiro - São Paulo, São Paulo - JARDIM PARQUE MORUMBI</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>(11) 98621-0785
-(11) 95857-6255</t>
+          <t>(11) 96254-1192
+(63) 98116-2486</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ellencarolinesilvaviana@gmail.com</t>
+          <t>gabrieltrevocardoso@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Kayane Rodrigues piovesan</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr"/>
+          <t>Andreza Pereira dos Santos</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>31 anos, Solteira - São Paulo, São Paulo - Jardim Helga</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>(11) 96564-1757</t>
+          <t>(11) 97677-9539</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>kayanelorennalucas@gmail.com</t>
+          <t>andrezapds@yahoo.com.br</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Guilherme Alves Monteiro De Souza</t>
+          <t>Wagner Coutinho da Silva</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>31 anos, Solteiro - São Paulo, São Paulo - PARQUE SAO PAULO</t>
+          <t>Casado - São Paulo, São Paulo - Vila Amalia</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>(11) 94264-9234
-(11) 5929-1988</t>
+          <t>(11) 96932-2690
+(11) 2554-1837</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>guilhermealves9420@gmail.com</t>
+          <t>wagner.coutinho93@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>clebison santos medeiros</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr"/>
+          <t>Maria Yasmin Soares da Silva</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>18 anos, Solteira - São Paulo, São Paulo - Cohab jardim Antártica</t>
+        </is>
+      </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>(11) 94353-5488</t>
+          <t>(11) 91320-6891</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>clebisonmedeiros9701@gmail.com</t>
+          <t>Mariayas2007@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Letycia Cardoso Pinto</t>
+          <t>Bianca Nunes</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>20 anos, Solteira - São Paulo, São Paulo - MOOCA</t>
+          <t>29 anos, Solteira - São Paulo, São Paulo - COHAB 2</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>(11) 98447-5562</t>
+          <t>(11) 97063-1415</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>letycia.cardosopinto2006@gmail.com</t>
+          <t>biahnunes2222@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Evelyne Falcao</t>
+          <t>ALINE LAUDICEIA COSTA DOS SANTOS</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>42 anos, Solteira - São Paulo, São Paulo - VILA OLIMPIA</t>
+          <t>37 anos, Divorciada - São Paulo, São Paulo - PARQUE BELEM</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>(21) 98361-4606</t>
+          <t>(11) 94947-7263</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>evelyne.marcato@gmail.com</t>
+          <t>aline.piceli25@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Monica Calado da Silva</t>
+          <t>Thauany Alessandra</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>30 anos, Solteira - São Paulo, São Paulo - Jardim Peri</t>
+          <t>18 anos, Solteira - São Paulo, São Paulo - Luis Botta</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>(11) 96135-3362
-(11) 93384-7260</t>
+          <t>(11) 97866-7864</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>monicaah.silva@gmail.com</t>
+          <t>eunany1984@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Caicque Pereira Magalhães</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
+          <t>Gabrielle Melo</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>São Paulo, São Paulo</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>(22) 99222-8476</t>
+          <t>(21) 98505-5276</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>caicquepmagalhaes@gmail.com</t>
+          <t>gmelo2608@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Thayane da Silva Moreira de Paula</t>
+          <t>Gabriel Moraes</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>27 anos, Divorciada - São Paulo, São Paulo - Casa Verde Alta</t>
+          <t>São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>(11) 96467-9534</t>
+          <t>(11) 91479-9682</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>thayanedepaula@outlook.com.br</t>
+          <t>jagaju.230426@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NERCI NASCIMENTO DA SILVA SANTOS</t>
+          <t>Naxiane Silva</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>58 anos, Casada - São Paulo, São Paulo - VILA JACUI</t>
+          <t>39 anos, Casada - São Paulo, São Paulo</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>(11) 96838-6389</t>
+          <t>(11) 94856-6295
+(11) 94856-6295</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>nercis.s@hotmail.com</t>
+          <t>naxianesilva@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>